<commit_message>
Actualizada documentacion de cableado
</commit_message>
<xml_diff>
--- a/docs/Conexion_Sensores.xlsx
+++ b/docs/Conexion_Sensores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ProMatix\Dropbox\TAREAS\secretaria\est_monit_rio_jachal\Software Datalogger\docs\Datalogger\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ProMatix\Dropbox\TAREAS\secretaria\est_monit_rio_jachal\Software Datalogger\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6FF7F1-269B-4C3F-83B1-195BC458231B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAE1E12-430C-417A-B5D7-58BF4ED42157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="62">
   <si>
     <t>Sensor</t>
   </si>
@@ -202,9 +202,6 @@
     <t>Rojo | Rojo</t>
   </si>
   <si>
-    <t>hilos</t>
-  </si>
-  <si>
     <t>CSIM11-PH-04L</t>
   </si>
   <si>
@@ -212,6 +209,12 @@
   </si>
   <si>
     <t>CS547a</t>
+  </si>
+  <si>
+    <t>hilos usados</t>
+  </si>
+  <si>
+    <t>Largo original [m]</t>
   </si>
 </sst>
 </file>
@@ -689,7 +692,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
@@ -722,6 +725,24 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -740,24 +761,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="17" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="20% - Énfasis6" xfId="5" builtinId="50"/>
@@ -769,41 +773,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -908,13 +877,46 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -922,12 +924,14 @@
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -974,12 +978,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D68336EB-A87B-42BD-B435-6661BA0DB120}" name="Tabla1" displayName="Tabla1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
-  <autoFilter ref="A1:C5" xr:uid="{D68336EB-A87B-42BD-B435-6661BA0DB120}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{26976802-83CA-417F-AC42-783A6355ED82}" name="Sensor" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{33FD598E-E3FB-4F60-B26B-F577D543B8EC}" name="modelo" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{592F1ABA-7AC0-4E12-8D1B-1A67F6B85355}" name="hilos" dataDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D68336EB-A87B-42BD-B435-6661BA0DB120}" name="Tabla1" displayName="Tabla1" ref="A1:D5" totalsRowShown="0" headerRowDxfId="6" headerRowBorderDxfId="5" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A1:D5" xr:uid="{D68336EB-A87B-42BD-B435-6661BA0DB120}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{26976802-83CA-417F-AC42-783A6355ED82}" name="Sensor" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{33FD598E-E3FB-4F60-B26B-F577D543B8EC}" name="modelo" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{592F1ABA-7AC0-4E12-8D1B-1A67F6B85355}" name="hilos usados" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{490A45A4-4D05-44C9-9093-81EAC34B75ED}" name="Largo original [m]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1218,7 +1223,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="28">
+      <c r="A2" s="46">
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1238,7 +1243,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+      <c r="A3" s="47"/>
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
@@ -1254,7 +1259,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="47"/>
       <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
@@ -1268,7 +1273,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1286,7 +1291,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="47"/>
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -1304,7 +1309,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="47"/>
       <c r="B7" s="2" t="s">
         <v>37</v>
       </c>
@@ -1320,7 +1325,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="47"/>
       <c r="B8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1336,7 +1341,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
+      <c r="A9" s="47"/>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
@@ -1352,7 +1357,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
+      <c r="A10" s="47"/>
       <c r="B10" s="2" t="s">
         <v>37</v>
       </c>
@@ -1366,7 +1371,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="47"/>
       <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1382,7 +1387,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="47"/>
       <c r="B12" s="2" t="s">
         <v>37</v>
       </c>
@@ -1398,7 +1403,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="47"/>
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
@@ -1414,7 +1419,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="47"/>
       <c r="B14" s="2" t="s">
         <v>37</v>
       </c>
@@ -1424,7 +1429,7 @@
       <c r="F14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="47"/>
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
@@ -1436,7 +1441,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="47"/>
       <c r="B16" s="2" t="s">
         <v>37</v>
       </c>
@@ -1450,7 +1455,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="3" t="s">
         <v>30</v>
       </c>
@@ -1460,7 +1465,7 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="29"/>
+      <c r="A18" s="47"/>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1470,7 +1475,7 @@
       <c r="F18" s="6"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="30"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="12" t="s">
         <v>36</v>
       </c>
@@ -1482,98 +1487,98 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="31">
+      <c r="A20" s="49">
         <v>2</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="5"/>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="37" t="s">
+      <c r="E20" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="29" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="38" t="s">
+      <c r="D21" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="38" t="s">
+      <c r="E21" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="36" t="s">
+      <c r="F21" s="30" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="3"/>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="34" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="28" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="41" t="s">
+      <c r="D23" s="35" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="17"/>
-      <c r="F23" s="39" t="s">
+      <c r="F23" s="33" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
+      <c r="A24" s="50"/>
       <c r="B24" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="3"/>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="34" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="34" t="s">
+      <c r="F24" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="42"/>
+      <c r="G24" s="36"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
+      <c r="A25" s="50"/>
       <c r="B25" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="34" t="s">
         <v>10</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="28" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
+      <c r="A26" s="50"/>
       <c r="B26" s="3" t="s">
         <v>17</v>
       </c>
@@ -1587,7 +1592,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="32"/>
+      <c r="A27" s="50"/>
       <c r="B27" s="3" t="s">
         <v>33</v>
       </c>
@@ -1597,7 +1602,7 @@
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="33"/>
+      <c r="A28" s="51"/>
       <c r="B28" s="17" t="s">
         <v>18</v>
       </c>
@@ -1644,72 +1649,88 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B02B97-FE78-4CAC-9594-3EDFA22D6A86}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.125" customWidth="1"/>
     <col min="2" max="2" width="14.125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="9.625" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="42">
+        <v>5</v>
+      </c>
+      <c r="D2" s="52">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="42">
+        <v>3</v>
+      </c>
+      <c r="D3" s="52">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="48">
+      <c r="C4" s="42">
+        <v>3</v>
+      </c>
+      <c r="D4" s="52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="45">
+        <v>3</v>
+      </c>
+      <c r="D5" s="52">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="48">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="51">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>